<commit_message>
Commit before changing all of the names
</commit_message>
<xml_diff>
--- a/symbols/My_Capacitor-1206.xlsx
+++ b/symbols/My_Capacitor-1206.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbwal\VSCode\KiCAD\electronics-library\symbols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250CF76C-6CD9-4848-A2F8-163CA19468E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBCB5E3-122A-48D7-A1D3-6F2788466DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52545" yWindow="915" windowWidth="24840" windowHeight="19965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="0" windowWidth="24840" windowHeight="19965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="~Template" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Symbol Name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>JLCPCB</t>
   </si>
   <si>
-    <t>JLCPCB Type</t>
-  </si>
-  <si>
     <t>C1846</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>cap capacitor basic</t>
-  </si>
-  <si>
-    <t>Basic</t>
   </si>
   <si>
     <t>1uF</t>
@@ -245,7 +239,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -550,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +557,7 @@
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,278 +579,245 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="str">
         <f>A2</f>
         <v>10nF</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B11" si="0">A3</f>
         <v>1uF</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>1nF</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>22uF</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>10uF</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>100uF</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>100nF</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>4.7uF</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>2.2uF</v>
       </c>
       <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>47uF</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>